<commit_message>
Created README files to describe the fast-spectrum benchmarks
</commit_message>
<xml_diff>
--- a/Benchmarks/originals/PU_MET_FAST_005/PU_MET_FAST_005.xlsx
+++ b/Benchmarks/originals/PU_MET_FAST_005/PU_MET_FAST_005.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\ML_neutronics\PU-MET-FAST-005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\ML_Nuclear_Data\Benchmarks\originals\PU_MET_FAST_005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03946796-2562-426C-A627-214B437502E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A0080D-DC7D-4845-8C4D-6CC5FB256ED3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2867" yWindow="3593" windowWidth="19200" windowHeight="10074" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -571,91 +571,91 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1031,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1046,47 +1046,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="50"/>
-      <c r="G1" s="44" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="63"/>
+      <c r="G1" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="45"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="51" t="s">
+      <c r="C2" s="65"/>
+      <c r="D2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="G2" s="46" t="s">
+      <c r="E2" s="65"/>
+      <c r="G2" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="47"/>
+      <c r="H2" s="60"/>
     </row>
     <row r="3" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="53" t="s">
+      <c r="C3" s="67"/>
+      <c r="D3" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="54"/>
+      <c r="E3" s="67"/>
       <c r="G3" s="15" t="s">
         <v>19</v>
       </c>
@@ -1098,14 +1098,14 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="55" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="56"/>
+      <c r="E4" s="47"/>
       <c r="G4" s="29" t="s">
         <v>9</v>
       </c>
@@ -1137,7 +1137,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="50" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="4">
@@ -1146,10 +1146,10 @@
       <c r="C6" s="5">
         <v>2.0600000000000002E-3</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="51">
         <v>1.008</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="53">
         <v>1E-3</v>
       </c>
       <c r="G6" s="17" t="s">
@@ -1160,15 +1160,15 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A7" s="37"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="6">
         <v>1.0102800000000001</v>
       </c>
       <c r="C7" s="7">
         <v>1.98E-3</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="40"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="53"/>
       <c r="G7" s="22" t="s">
         <v>26</v>
       </c>
@@ -1177,15 +1177,15 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="37"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="6">
         <v>2.0591400000000001E-3</v>
       </c>
       <c r="C8" s="7">
         <v>4.9410000000000003E-2</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="40"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="53"/>
       <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
@@ -1203,12 +1203,12 @@
       <c r="C9" s="7">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="40"/>
-      <c r="G9" s="46" t="s">
+      <c r="D9" s="51"/>
+      <c r="E9" s="53"/>
+      <c r="G9" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="47"/>
+      <c r="H9" s="60"/>
     </row>
     <row r="10" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8" t="s">
@@ -1220,8 +1220,8 @@
       <c r="C10" s="7">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="40"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="53"/>
       <c r="G10" s="15" t="s">
         <v>19</v>
       </c>
@@ -1239,8 +1239,8 @@
       <c r="C11" s="7">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="41"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="54"/>
       <c r="G11" s="31" t="s">
         <v>9</v>
       </c>
@@ -1266,7 +1266,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="55" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="10">
@@ -1283,7 +1283,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A14" s="42"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="10">
         <v>1</v>
       </c>
@@ -1298,7 +1298,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="43"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="13">
         <v>1</v>
       </c>
@@ -1314,125 +1314,110 @@
     </row>
     <row r="16" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="17" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="43"/>
     </row>
     <row r="18" spans="1:5" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="60" t="s">
+      <c r="C18" s="45"/>
+      <c r="D18" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="61"/>
+      <c r="E18" s="45"/>
     </row>
     <row r="19" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="55" t="s">
+      <c r="C19" s="47"/>
+      <c r="D19" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="56"/>
+      <c r="E19" s="47"/>
     </row>
     <row r="20" spans="1:5" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A20" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="63"/>
-      <c r="D20" s="62" t="s">
+      <c r="C20" s="49"/>
+      <c r="D20" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="63"/>
+      <c r="E20" s="49"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="64">
+      <c r="B21" s="37">
         <v>5000</v>
       </c>
-      <c r="C21" s="65"/>
-      <c r="D21" s="64">
-        <v>1500</v>
-      </c>
-      <c r="E21" s="65"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="37">
+        <v>1000</v>
+      </c>
+      <c r="E21" s="38"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="64">
+      <c r="B22" s="37">
         <v>100</v>
       </c>
-      <c r="C22" s="65"/>
-      <c r="D22" s="64">
+      <c r="C22" s="38"/>
+      <c r="D22" s="37">
         <v>310</v>
       </c>
-      <c r="E22" s="65"/>
+      <c r="E22" s="38"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="64">
+      <c r="B23" s="37">
         <v>20</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="64">
+      <c r="C23" s="38"/>
+      <c r="D23" s="37">
         <v>10</v>
       </c>
-      <c r="E23" s="65"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="24" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="66">
+      <c r="B24" s="39">
         <f>B21*(B22-B23)</f>
         <v>400000</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="66">
+      <c r="C24" s="40"/>
+      <c r="D24" s="39">
         <f>D21*(D22-D23)</f>
-        <v>450000</v>
-      </c>
-      <c r="E24" s="67"/>
+        <v>300000</v>
+      </c>
+      <c r="E24" s="40"/>
     </row>
     <row r="25" spans="1:5" ht="14.7" thickTop="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="D6:D11"/>
     <mergeCell ref="E6:E11"/>
@@ -1447,6 +1432,21 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>